<commit_message>
update phone number detection logic
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -466,17 +466,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>+966504435170</t>
+          <t>+966558927634</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>كلموني اخر ٢٤ ساعه</t>
+          <t>كلموني اخر ٢٤ ساعه, +966 55 892 7634</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Sunday 4:08</t>
+          <t>Sunday</t>
         </is>
       </c>
     </row>
@@ -488,17 +488,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>+966590423200</t>
+          <t>+966531482587</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>كلموني اخر ٢٤ ساعه</t>
+          <t>كلموني اخر ٢٤ ساعه, +966 55 892 7634</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Sunday 4:08</t>
+          <t>Sunday</t>
         </is>
       </c>
     </row>
@@ -510,17 +510,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>+966566626124</t>
+          <t>+966594320944</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>كلموني اخر ٢٤ ساعه</t>
+          <t>كلموني اخر ٢٤ ساعه, +966 55 892 7634</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Sunday 4:08</t>
+          <t>Sunday</t>
         </is>
       </c>
     </row>
@@ -532,17 +532,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>+966537394446</t>
+          <t>+966504435170</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>كلموني اخر ٢٤ ساعه</t>
+          <t>كلموني اخر ٢٤ ساعه, +966 55 892 7634</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Sunday 4:08</t>
+          <t>Sunday</t>
         </is>
       </c>
     </row>
@@ -554,17 +554,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>+966594320944</t>
+          <t>+966552914008</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>كلموني اخر ٢٤ ساعه</t>
+          <t>كلموني اخر ٢٤ ساعه, +966 55 892 7634</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Sunday 4:08</t>
+          <t>Sunday</t>
         </is>
       </c>
     </row>
@@ -576,17 +576,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>+966531482587</t>
+          <t>+966590423200</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>كلموني اخر ٢٤ ساعه</t>
+          <t>كلموني اخر ٢٤ ساعه, +966 55 892 7634</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Sunday 4:08</t>
+          <t>Sunday</t>
         </is>
       </c>
     </row>
@@ -598,17 +598,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>+966536276067</t>
+          <t>+966566626124</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>كلموني اخر ٢٤ ساعه</t>
+          <t>كلموني اخر ٢٤ ساعه, +966 55 892 7634</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Sunday 4:08</t>
+          <t>Sunday</t>
         </is>
       </c>
     </row>
@@ -620,17 +620,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>+966558927634</t>
+          <t>+966537394446</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>كلموني اخر ٢٤ ساعه</t>
+          <t>كلموني اخر ٢٤ ساعه, +966 55 892 7634</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Sunday 4:08</t>
+          <t>Sunday</t>
         </is>
       </c>
     </row>
@@ -642,17 +642,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>+966552914008</t>
+          <t>+966536276067</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>كلموني اخر ٢٤ ساعه</t>
+          <t>كلموني اخر ٢٤ ساعه, +966 55 892 7634</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Sunday 4:08</t>
+          <t>Sunday</t>
         </is>
       </c>
     </row>
@@ -802,12 +802,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>كلموني اخر ٢٤ ساعه</t>
+          <t>كلموني اخر ٢٤ ساعه, +966 55 892 7634</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Sunday 4:08</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="E2" t="n">

</xml_diff>

<commit_message>
only detect phone number
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -9,8 +9,7 @@
   <sheets>
     <sheet name="Phone Numbers" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Unique Numbers" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Summary" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="All Text" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="All Text" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -428,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,16 +446,6 @@
           <t>Phone_Number</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Timestamp</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -469,16 +458,6 @@
           <t>+966558927634</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>كلموني اخر ٢٤ ساعه, +966 55 892 7634</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Sunday</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -491,16 +470,6 @@
           <t>+966531482587</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>كلموني اخر ٢٤ ساعه, +966 55 892 7634</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Sunday</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -513,16 +482,6 @@
           <t>+966594320944</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>كلموني اخر ٢٤ ساعه, +966 55 892 7634</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Sunday</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -535,16 +494,6 @@
           <t>+966504435170</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>كلموني اخر ٢٤ ساعه, +966 55 892 7634</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Sunday</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -557,16 +506,6 @@
           <t>+966552914008</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>كلموني اخر ٢٤ ساعه, +966 55 892 7634</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Sunday</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -579,16 +518,6 @@
           <t>+966590423200</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>كلموني اخر ٢٤ ساعه, +966 55 892 7634</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Sunday</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -601,16 +530,6 @@
           <t>+966566626124</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>كلموني اخر ٢٤ ساعه, +966 55 892 7634</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Sunday</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -623,16 +542,6 @@
           <t>+966537394446</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>كلموني اخر ٢٤ ساعه, +966 55 892 7634</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Sunday</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -643,16 +552,6 @@
       <c r="B10" t="inlineStr">
         <is>
           <t>+966536276067</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>كلموني اخر ٢٤ ساعه, +966 55 892 7634</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Sunday</t>
         </is>
       </c>
     </row>
@@ -756,7 +655,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -772,22 +671,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Phone_Numbers_Count</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Names_Detected</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Timestamp</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Text_Blocks_Count</t>
+          <t>All_Extracted_Text</t>
         </is>
       </c>
     </row>
@@ -797,73 +681,9 @@
           <t>1.png</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>9</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>كلموني اخر ٢٤ ساعه, +966 55 892 7634</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Sunday</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Image_Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>All_Extracted_Text</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Arabic_Messages</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1.png</t>
-        </is>
-      </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>4:08 39 كلموني اخر ٢٤ ساعه Edit +966 55 892 7634 Sunday كلمتنا وعندك اهتمام اذا ٠9. الله كلموني اخر ٢٤ ساعه +966 53 148 2587 Sunday الله محييكم كلمتنا وعندك اهتمام اذا ٠9. كلموني اخر ٢٤ ساعه +966 59 432 0944 Sunday كلمتنا وعندك اهتمام اذا ٠9. الله كلموني اخر ٢٤ ساعه +966 50 443 5170 Sunday الله محييكم كلمتنا وعندك اهتمام اذا ٠9. اخر ٢٤ ساعه كلموني +966 55 291 4008 Sunday كلمتنا وعندك اهتمام اذا 9.. الله كلموني اخر ٢٤ ساعه +966 59 042 3200 Sunday الله محييكم كلمتنا وعندك اهتمام اذا ٠9. كلموني اخر ٢٤ ساعه +966 56 662 6124 Sunday الله محييكم كلمتنا وعندك اهتمام اذا ٠9. اخر ٢٤ ساعه كلموني +966 53 739 4446 Sunday وتلئ رب الله محييكم كلمتنا وعندك اهتمام اذا ٠9. كلموني اخر ٢٤ ساعه +966 53 627 6067 Sunday الله محييكم كلمتنا معندك اهتمام اذا ٠٠9. محييكم محييكم محييكم</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>كلموني اخر ٢٤ ساعه | كلمتنا وعندك اهتمام اذا ٠ | الله كلموني اخر ٢٤ ساعه | الله محييكم كلمتنا وعندك اهتمام اذا ٠ | كلموني اخر ٢٤ ساعه | كلمتنا وعندك اهتمام اذا ٠ | الله كلموني اخر ٢٤ ساعه | الله محييكم كلمتنا وعندك اهتمام اذا ٠ | اخر ٢٤ ساعه كلموني | كلمتنا وعندك اهتمام اذا | الله كلموني اخر ٢٤ ساعه | الله محييكم كلمتنا وعندك اهتمام اذا ٠ | كلموني اخر ٢٤ ساعه | الله محييكم كلمتنا وعندك اهتمام اذا ٠ | اخر ٢٤ ساعه كلموني | وتلئ رب الله محييكم كلمتنا وعندك اهتمام اذا ٠ | كلموني اخر ٢٤ ساعه | الله محييكم كلمتنا معندك اهتمام اذا ٠٠ | محييكم محييكم محييكم</t>
         </is>
       </c>
     </row>

</xml_diff>